<commit_message>
Points update sysy kol2
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jczec\Pulpit\IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE925AE0-6BC7-45EE-ADE6-8F7E3C664EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15913544-CB26-4109-B429-4DF69BC58E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="I-semestr-24Z" sheetId="2" r:id="rId1"/>
@@ -1179,9 +1179,18 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1191,10 +1200,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1203,17 +1215,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1246,24 +1264,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1629,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5356A30-E1AA-4069-A4C8-FC0BE8204C56}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V45" sqref="V45"/>
     </sheetView>
   </sheetViews>
@@ -1695,23 +1695,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="51"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1793,28 +1793,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="45"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="50">
+      <c r="B10" s="46">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="E10" s="51">
+      <c r="C10" s="46"/>
+      <c r="E10" s="55">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="E11" s="52"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="E11" s="56"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1859,20 +1859,20 @@
       <c r="H15" s="44"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="F17" s="45" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="F17" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="J17" s="49" t="s">
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="J17" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="49"/>
+      <c r="K17" s="45"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1896,12 +1896,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="50">
+      <c r="J18" s="46">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="50"/>
-      <c r="M18" s="54">
+      <c r="K18" s="46"/>
+      <c r="M18" s="48">
         <v>5</v>
       </c>
     </row>
@@ -1924,9 +1924,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="M19" s="54"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="M19" s="48"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1977,20 +1977,20 @@
       <c r="K24" s="44"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="E26" s="46" t="s">
+      <c r="C26" s="47"/>
+      <c r="E26" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48"/>
-      <c r="I26" s="45" t="s">
+      <c r="F26" s="50"/>
+      <c r="G26" s="51"/>
+      <c r="I26" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2025,12 +2025,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="53">
+      <c r="M27" s="54">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="54">
+      <c r="O27" s="48">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2060,9 +2060,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="53"/>
+      <c r="M28" s="54"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="54"/>
+      <c r="O28" s="48"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2110,17 +2110,17 @@
       <c r="I33" s="44"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="45"/>
-      <c r="D35" s="45"/>
-      <c r="F35" s="45" t="s">
+      <c r="C35" s="47"/>
+      <c r="D35" s="47"/>
+      <c r="F35" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -2177,14 +2177,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="F40" s="50" t="s">
+      <c r="C40" s="53"/>
+      <c r="F40" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="50"/>
+      <c r="G40" s="46"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2240,7 +2240,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="49" t="s">
+      <c r="I43" s="45" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="49"/>
+      <c r="I44" s="45"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2441,27 +2441,27 @@
       <c r="R59" s="44"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="45" t="s">
+      <c r="B61" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45"/>
-      <c r="E61" s="45"/>
-      <c r="F61" s="45"/>
-      <c r="G61" s="45"/>
-      <c r="H61" s="45"/>
-      <c r="I61" s="45"/>
-      <c r="J61" s="45"/>
-      <c r="K61" s="45"/>
-      <c r="M61" s="45" t="s">
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="M61" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="45"/>
-      <c r="O61" s="45"/>
-      <c r="Q61" s="45" t="s">
+      <c r="N61" s="47"/>
+      <c r="O61" s="47"/>
+      <c r="Q61" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="45"/>
+      <c r="R61" s="47"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2558,28 +2558,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="49" t="s">
+      <c r="B66" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="49"/>
+      <c r="C66" s="45"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="50">
+      <c r="B67" s="46">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="50"/>
-      <c r="E67" s="54">
+      <c r="C67" s="46"/>
+      <c r="E67" s="48">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="50"/>
-      <c r="C68" s="50"/>
-      <c r="E68" s="54"/>
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="E68" s="48"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -2650,10 +2650,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="49" t="s">
+      <c r="K75" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="49"/>
+      <c r="L75" s="45"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -2683,11 +2683,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="50">
+      <c r="K76" s="46">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="50"/>
+      <c r="L76" s="46"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -2715,6 +2715,30 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="B23:K24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="F35:I35"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="F40:G40"/>
     <mergeCell ref="B72:I73"/>
     <mergeCell ref="K75:L75"/>
     <mergeCell ref="K76:L76"/>
@@ -2725,30 +2749,6 @@
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B67:C68"/>
     <mergeCell ref="E67:E68"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="B23:K24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="F35:I35"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2759,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,60 +2789,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="59"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="65"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="62"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="68"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="48"/>
-      <c r="H5" s="46" t="s">
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
+      <c r="H5" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="K5" s="46" t="s">
+      <c r="I5" s="51"/>
+      <c r="K5" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="48"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="51"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2918,37 +2918,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="49"/>
+      <c r="C9" s="45"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="49" t="s">
+      <c r="G9" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="49"/>
+      <c r="H9" s="45"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="50">
+      <c r="B10" s="46">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>29.9</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="G10" s="50">
+      <c r="C10" s="46"/>
+      <c r="E10" s="55"/>
+      <c r="G10" s="46">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>36.1</v>
       </c>
-      <c r="H10" s="50"/>
+      <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="E11" s="52"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="E11" s="56"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2973,46 +2973,46 @@
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="58"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="59"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="60"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="62"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="68"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="H17" s="46" t="s">
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="H17" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="47"/>
-      <c r="J17" s="48"/>
-      <c r="L17" s="49" t="s">
+      <c r="I17" s="50"/>
+      <c r="J17" s="51"/>
+      <c r="L17" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="49"/>
-      <c r="O17" s="49" t="s">
+      <c r="M17" s="45"/>
+      <c r="O17" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="49"/>
+      <c r="P17" s="45"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3042,17 +3042,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="50">
+      <c r="L18" s="46">
         <f>SUM(B19:F19,H19:J19)</f>
-        <v>34.5</v>
-      </c>
-      <c r="M18" s="50"/>
-      <c r="O18" s="50">
+        <v>47</v>
+      </c>
+      <c r="M18" s="46"/>
+      <c r="O18" s="46">
         <f>50-SUM(B19:F19,H19:J19)</f>
-        <v>15.5</v>
-      </c>
-      <c r="P18" s="50"/>
-      <c r="R18" s="54"/>
+        <v>3</v>
+      </c>
+      <c r="P18" s="46"/>
+      <c r="R18" s="48"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
@@ -3068,12 +3068,14 @@
       <c r="I19" s="2">
         <v>21</v>
       </c>
-      <c r="J19" s="2"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="50"/>
-      <c r="O19" s="50"/>
-      <c r="P19" s="50"/>
-      <c r="R19" s="54"/>
+      <c r="J19" s="2">
+        <v>12.5</v>
+      </c>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="R19" s="48"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3098,56 +3100,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="58"/>
-      <c r="L23" s="59"/>
-      <c r="N23" s="50" t="s">
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="65"/>
+      <c r="N23" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="50"/>
+      <c r="O23" s="46"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="62"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="50"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="68"/>
+      <c r="N24" s="46"/>
+      <c r="O24" s="46"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="F26" s="45" t="s">
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="F26" s="47" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="46" t="s">
+      <c r="K26" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="48"/>
+      <c r="L26" s="51"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -3180,7 +3182,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="51"/>
+      <c r="N27" s="55"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -3204,7 +3206,7 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="52"/>
+      <c r="N28" s="56"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -3229,39 +3231,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="70"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="71"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="73"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="62"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="45" t="s">
+      <c r="B35" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="45"/>
+      <c r="C35" s="47"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="46" t="s">
+      <c r="E35" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="48"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50"/>
+      <c r="H35" s="51"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -3304,14 +3306,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="56"/>
-      <c r="F40" s="50" t="s">
+      <c r="C40" s="53"/>
+      <c r="F40" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="50"/>
+      <c r="G40" s="46"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3365,7 +3367,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="49" t="s">
+      <c r="I43" s="45" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3380,7 +3382,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="49"/>
+      <c r="I44" s="45"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3519,70 +3521,70 @@
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="57" t="s">
+      <c r="B60" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
-      <c r="K60" s="58"/>
-      <c r="L60" s="58"/>
-      <c r="M60" s="58"/>
-      <c r="N60" s="58"/>
-      <c r="O60" s="58"/>
-      <c r="P60" s="58"/>
-      <c r="Q60" s="58"/>
-      <c r="R60" s="58"/>
-      <c r="S60" s="59"/>
+      <c r="C60" s="64"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="64"/>
+      <c r="F60" s="64"/>
+      <c r="G60" s="64"/>
+      <c r="H60" s="64"/>
+      <c r="I60" s="64"/>
+      <c r="J60" s="64"/>
+      <c r="K60" s="64"/>
+      <c r="L60" s="64"/>
+      <c r="M60" s="64"/>
+      <c r="N60" s="64"/>
+      <c r="O60" s="64"/>
+      <c r="P60" s="64"/>
+      <c r="Q60" s="64"/>
+      <c r="R60" s="64"/>
+      <c r="S60" s="65"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="60"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="61"/>
-      <c r="K61" s="61"/>
-      <c r="L61" s="61"/>
-      <c r="M61" s="61"/>
-      <c r="N61" s="61"/>
-      <c r="O61" s="61"/>
-      <c r="P61" s="61"/>
-      <c r="Q61" s="61"/>
-      <c r="R61" s="61"/>
-      <c r="S61" s="62"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="67"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="67"/>
+      <c r="F61" s="67"/>
+      <c r="G61" s="67"/>
+      <c r="H61" s="67"/>
+      <c r="I61" s="67"/>
+      <c r="J61" s="67"/>
+      <c r="K61" s="67"/>
+      <c r="L61" s="67"/>
+      <c r="M61" s="67"/>
+      <c r="N61" s="67"/>
+      <c r="O61" s="67"/>
+      <c r="P61" s="67"/>
+      <c r="Q61" s="67"/>
+      <c r="R61" s="67"/>
+      <c r="S61" s="68"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="45" t="s">
+      <c r="B63" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="45"/>
-      <c r="D63" s="45"/>
-      <c r="E63" s="45"/>
-      <c r="F63" s="45"/>
-      <c r="G63" s="45"/>
-      <c r="H63" s="45"/>
-      <c r="I63" s="45"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="45"/>
-      <c r="M63" s="45" t="s">
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="47"/>
+      <c r="M63" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="45"/>
-      <c r="O63" s="45"/>
-      <c r="P63" s="45"/>
-      <c r="R63" s="45" t="s">
+      <c r="N63" s="47"/>
+      <c r="O63" s="47"/>
+      <c r="P63" s="47"/>
+      <c r="R63" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="45"/>
+      <c r="S63" s="47"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -3682,65 +3684,43 @@
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="49" t="s">
+      <c r="B68" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="49"/>
+      <c r="C68" s="45"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="49" t="s">
+      <c r="G68" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="49"/>
+      <c r="H68" s="45"/>
       <c r="J68" s="1">
         <v>4.5</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="50">
+      <c r="B69" s="46">
         <f>SUM(B65:K65,M65:P65,R65:S65)+J68</f>
         <v>34.5</v>
       </c>
-      <c r="C69" s="50"/>
-      <c r="E69" s="54"/>
-      <c r="G69" s="50">
+      <c r="C69" s="46"/>
+      <c r="E69" s="48"/>
+      <c r="G69" s="46">
         <f>50-SUM(B65:K65,M65:P65,R65:S65,J68)</f>
         <v>15.5</v>
       </c>
-      <c r="H69" s="50"/>
+      <c r="H69" s="46"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="E70" s="54"/>
-      <c r="G70" s="50"/>
-      <c r="H70" s="50"/>
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+      <c r="E70" s="48"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -3757,6 +3737,28 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4280,21 +4282,21 @@
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:12" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="69" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="F2" s="63" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="71"/>
+      <c r="F2" s="69" t="s">
         <v>204</v>
       </c>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-      <c r="J2" s="63" t="s">
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
+      <c r="J2" s="69" t="s">
         <v>205</v>
       </c>
-      <c r="K2" s="64"/>
-      <c r="L2" s="65"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34" t="s">
@@ -4469,26 +4471,26 @@
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="73"/>
       <c r="D11" s="33">
         <f>(D4*C4+D5*C5+D6*C6+D7*C7+D8*C8+D9*C9)/30</f>
         <v>3.9666666666666668</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="G11" s="67"/>
+      <c r="G11" s="73"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
         <v>0</v>
       </c>
-      <c r="J11" s="66" t="s">
+      <c r="J11" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="K11" s="67"/>
+      <c r="K11" s="73"/>
       <c r="L11" s="33">
         <f>(L4*K4+L5*K5+L6*K6+L7*K7+L8*K8)/30</f>
         <v>0</v>

</xml_diff>

<commit_message>
points and grades update
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jczec\Pulpit\IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15913544-CB26-4109-B429-4DF69BC58E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D467E8-FE92-4E96-A94F-0DD80F00B8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15285" activeTab="3" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="I-semestr-24Z" sheetId="2" r:id="rId1"/>
@@ -1179,40 +1179,58 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1231,24 +1249,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1695,23 +1695,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1793,28 +1793,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="50">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="55">
+      <c r="C10" s="50"/>
+      <c r="E10" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="56"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1859,20 +1859,20 @@
       <c r="H15" s="44"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="F17" s="47" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="F17" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="J17" s="45" t="s">
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="J17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="45"/>
+      <c r="K17" s="49"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1896,12 +1896,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="46">
+      <c r="J18" s="50">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="M18" s="48">
+      <c r="K18" s="50"/>
+      <c r="M18" s="54">
         <v>5</v>
       </c>
     </row>
@@ -1924,9 +1924,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="M19" s="48"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="M19" s="54"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1977,20 +1977,20 @@
       <c r="K24" s="44"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="E26" s="49" t="s">
+      <c r="C26" s="45"/>
+      <c r="E26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="51"/>
-      <c r="I26" s="47" t="s">
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="I26" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2025,12 +2025,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="54">
+      <c r="M27" s="53">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="48">
+      <c r="O27" s="54">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2060,9 +2060,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="54"/>
+      <c r="M28" s="53"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="48"/>
+      <c r="O28" s="54"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2110,17 +2110,17 @@
       <c r="I33" s="44"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="F35" s="47" t="s">
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="F35" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -2177,14 +2177,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="F40" s="46" t="s">
+      <c r="C40" s="56"/>
+      <c r="F40" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="46"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2240,7 +2240,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="45" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="45"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2441,27 +2441,27 @@
       <c r="R59" s="44"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="47" t="s">
+      <c r="B61" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="47"/>
-      <c r="M61" s="47" t="s">
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="45"/>
+      <c r="M61" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="47"/>
-      <c r="O61" s="47"/>
-      <c r="Q61" s="47" t="s">
+      <c r="N61" s="45"/>
+      <c r="O61" s="45"/>
+      <c r="Q61" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="47"/>
+      <c r="R61" s="45"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2558,28 +2558,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="45"/>
+      <c r="C66" s="49"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="46">
+      <c r="B67" s="50">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="E67" s="48">
+      <c r="C67" s="50"/>
+      <c r="E67" s="54">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="E68" s="48"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="E68" s="54"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -2650,10 +2650,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="45" t="s">
+      <c r="K75" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="45"/>
+      <c r="L75" s="49"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -2683,11 +2683,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="46">
+      <c r="K76" s="50">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="46"/>
+      <c r="L76" s="50"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -2715,20 +2715,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -2739,16 +2735,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2759,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P73" sqref="P73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,60 +2789,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="65"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="59"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="68"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="62"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="H5" s="49" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="H5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="K5" s="49" t="s">
+      <c r="I5" s="48"/>
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2918,37 +2918,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="45"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="50">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>29.9</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="55"/>
-      <c r="G10" s="46">
+      <c r="C10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="G10" s="50">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>36.1</v>
       </c>
-      <c r="H10" s="46"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="56"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="52"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2972,7 +2972,7 @@
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="63" t="s">
         <v>77</v>
       </c>
@@ -2981,38 +2981,38 @@
       <c r="E14" s="64"/>
       <c r="F14" s="64"/>
       <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="64"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
       <c r="D15" s="67"/>
       <c r="E15" s="67"/>
       <c r="F15" s="67"/>
       <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+      <c r="H15" s="67"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="H17" s="49" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="H17" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
-      <c r="L17" s="45" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="48"/>
+      <c r="L17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="45"/>
-      <c r="O17" s="45" t="s">
+      <c r="M17" s="49"/>
+      <c r="O17" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="45"/>
+      <c r="P17" s="49"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3042,25 +3042,33 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="50">
         <f>SUM(B19:F19,H19:J19)</f>
-        <v>47</v>
-      </c>
-      <c r="M18" s="46"/>
-      <c r="O18" s="46">
+        <v>70</v>
+      </c>
+      <c r="M18" s="50"/>
+      <c r="O18" s="50">
         <f>50-SUM(B19:F19,H19:J19)</f>
-        <v>3</v>
-      </c>
-      <c r="P18" s="46"/>
-      <c r="R18" s="48"/>
+        <v>-20</v>
+      </c>
+      <c r="P18" s="50"/>
+      <c r="R18" s="54">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>7</v>
+      </c>
       <c r="C19" s="2">
         <v>7</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>8</v>
+      </c>
       <c r="F19" s="2">
         <v>6.5</v>
       </c>
@@ -3071,11 +3079,11 @@
       <c r="J19" s="2">
         <v>12.5</v>
       </c>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="R19" s="48"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="R19" s="54"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3100,56 +3108,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="65"/>
-      <c r="N23" s="46" t="s">
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="59"/>
+      <c r="N23" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="46"/>
+      <c r="O23" s="50"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="66"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="68"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="62"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="F26" s="47" t="s">
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="F26" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="49" t="s">
+      <c r="K26" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="51"/>
+      <c r="L26" s="48"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -3182,7 +3190,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="55"/>
+      <c r="N27" s="51"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -3206,7 +3214,7 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="56"/>
+      <c r="N28" s="52"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -3231,39 +3239,39 @@
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B32" s="57" t="s">
+      <c r="B32" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="H32" s="64"/>
+      <c r="I32" s="65"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="67"/>
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="47"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="51"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -3306,14 +3314,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="F40" s="46" t="s">
+      <c r="C40" s="56"/>
+      <c r="F40" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="46"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3367,7 +3375,7 @@
         <v>119</v>
       </c>
       <c r="G43" s="2"/>
-      <c r="I43" s="45" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3382,7 +3390,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="45"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3521,70 +3529,70 @@
     </row>
     <row r="59" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="63" t="s">
+      <c r="B60" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="64"/>
-      <c r="D60" s="64"/>
-      <c r="E60" s="64"/>
-      <c r="F60" s="64"/>
-      <c r="G60" s="64"/>
-      <c r="H60" s="64"/>
-      <c r="I60" s="64"/>
-      <c r="J60" s="64"/>
-      <c r="K60" s="64"/>
-      <c r="L60" s="64"/>
-      <c r="M60" s="64"/>
-      <c r="N60" s="64"/>
-      <c r="O60" s="64"/>
-      <c r="P60" s="64"/>
-      <c r="Q60" s="64"/>
-      <c r="R60" s="64"/>
-      <c r="S60" s="65"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="58"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="58"/>
+      <c r="I60" s="58"/>
+      <c r="J60" s="58"/>
+      <c r="K60" s="58"/>
+      <c r="L60" s="58"/>
+      <c r="M60" s="58"/>
+      <c r="N60" s="58"/>
+      <c r="O60" s="58"/>
+      <c r="P60" s="58"/>
+      <c r="Q60" s="58"/>
+      <c r="R60" s="58"/>
+      <c r="S60" s="59"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="66"/>
-      <c r="C61" s="67"/>
-      <c r="D61" s="67"/>
-      <c r="E61" s="67"/>
-      <c r="F61" s="67"/>
-      <c r="G61" s="67"/>
-      <c r="H61" s="67"/>
-      <c r="I61" s="67"/>
-      <c r="J61" s="67"/>
-      <c r="K61" s="67"/>
-      <c r="L61" s="67"/>
-      <c r="M61" s="67"/>
-      <c r="N61" s="67"/>
-      <c r="O61" s="67"/>
-      <c r="P61" s="67"/>
-      <c r="Q61" s="67"/>
-      <c r="R61" s="67"/>
-      <c r="S61" s="68"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="61"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="61"/>
+      <c r="J61" s="61"/>
+      <c r="K61" s="61"/>
+      <c r="L61" s="61"/>
+      <c r="M61" s="61"/>
+      <c r="N61" s="61"/>
+      <c r="O61" s="61"/>
+      <c r="P61" s="61"/>
+      <c r="Q61" s="61"/>
+      <c r="R61" s="61"/>
+      <c r="S61" s="62"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="47" t="s">
+      <c r="B63" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="47"/>
-      <c r="M63" s="47" t="s">
+      <c r="C63" s="45"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="45"/>
+      <c r="M63" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="47"/>
-      <c r="O63" s="47"/>
-      <c r="P63" s="47"/>
-      <c r="R63" s="47" t="s">
+      <c r="N63" s="45"/>
+      <c r="O63" s="45"/>
+      <c r="P63" s="45"/>
+      <c r="R63" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="47"/>
+      <c r="S63" s="45"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -3684,43 +3692,65 @@
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="45" t="s">
+      <c r="B68" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="45"/>
+      <c r="C68" s="49"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="45" t="s">
+      <c r="G68" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="45"/>
+      <c r="H68" s="49"/>
       <c r="J68" s="1">
         <v>4.5</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="46">
+      <c r="B69" s="50">
         <f>SUM(B65:K65,M65:P65,R65:S65)+J68</f>
         <v>34.5</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="E69" s="48"/>
-      <c r="G69" s="46">
+      <c r="C69" s="50"/>
+      <c r="E69" s="54"/>
+      <c r="G69" s="50">
         <f>50-SUM(B65:K65,M65:P65,R65:S65,J68)</f>
         <v>15.5</v>
       </c>
-      <c r="H69" s="46"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
-      <c r="E70" s="48"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="46"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="E70" s="54"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -3737,28 +3767,6 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4263,8 +4271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA352BE-3E69-4CCA-8EEB-A9094B74606F}">
   <dimension ref="B1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="145" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4393,7 +4401,9 @@
       <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
       <c r="J6" s="38" t="s">
         <v>200</v>
       </c>
@@ -4485,7 +4495,7 @@
       <c r="G11" s="73"/>
       <c r="H11" s="33">
         <f>(H4*G4+H5*G5+H6*G6+H7*G7+H8*G8)/30</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J11" s="72" t="s">
         <v>197</v>

</xml_diff>

<commit_message>
Change in points file
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jczec\Pulpit\IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED729DB3-B531-4C6D-8431-0E9640C57044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D7F064-C2E0-466B-9A61-FE72DD19DFF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2070" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="I-semestr-24Z" sheetId="2" r:id="rId1"/>
@@ -691,7 +691,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-415]d\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -745,8 +745,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,8 +798,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -1035,11 +1049,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1179,78 +1209,78 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1266,8 +1296,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Dane wyjściowe" xfId="1" builtinId="21"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1695,23 +1729,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="49" t="s">
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1793,28 +1827,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="50">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>110</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="55">
+      <c r="C10" s="50"/>
+      <c r="E10" s="51">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="56"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="52"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1859,20 +1893,20 @@
       <c r="H15" s="44"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="F17" s="47" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="F17" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="J17" s="45" t="s">
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="J17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="45"/>
+      <c r="K17" s="49"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1896,12 +1930,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="46">
+      <c r="J18" s="50">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>93</v>
       </c>
-      <c r="K18" s="46"/>
-      <c r="M18" s="48">
+      <c r="K18" s="50"/>
+      <c r="M18" s="54">
         <v>5</v>
       </c>
     </row>
@@ -1924,9 +1958,9 @@
       <c r="H19" s="2">
         <v>4</v>
       </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="M19" s="48"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="M19" s="54"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -1977,20 +2011,20 @@
       <c r="K24" s="44"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="E26" s="49" t="s">
+      <c r="C26" s="45"/>
+      <c r="E26" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="51"/>
-      <c r="I26" s="47" t="s">
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
+      <c r="I26" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
+      <c r="J26" s="45"/>
+      <c r="K26" s="45"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2025,12 +2059,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="54">
+      <c r="M27" s="53">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>36</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="48">
+      <c r="O27" s="54">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2060,9 +2094,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="54"/>
+      <c r="M28" s="53"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="48"/>
+      <c r="O28" s="54"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2110,17 +2144,17 @@
       <c r="I33" s="44"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="47"/>
-      <c r="F35" s="47" t="s">
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="F35" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -2177,14 +2211,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="F40" s="46" t="s">
+      <c r="C40" s="56"/>
+      <c r="F40" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="46"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2240,7 +2274,7 @@
       <c r="G43" s="2">
         <v>0.44</v>
       </c>
-      <c r="I43" s="45" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2257,7 +2291,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="45"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2441,27 +2475,27 @@
       <c r="R59" s="44"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="47" t="s">
+      <c r="B61" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="47"/>
-      <c r="M61" s="47" t="s">
+      <c r="C61" s="45"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="45"/>
+      <c r="I61" s="45"/>
+      <c r="J61" s="45"/>
+      <c r="K61" s="45"/>
+      <c r="M61" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="47"/>
-      <c r="O61" s="47"/>
-      <c r="Q61" s="47" t="s">
+      <c r="N61" s="45"/>
+      <c r="O61" s="45"/>
+      <c r="Q61" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="47"/>
+      <c r="R61" s="45"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2558,28 +2592,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="45" t="s">
+      <c r="B66" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="45"/>
+      <c r="C66" s="49"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="46">
+      <c r="B67" s="50">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>85.5</v>
       </c>
-      <c r="C67" s="46"/>
-      <c r="E67" s="48">
+      <c r="C67" s="50"/>
+      <c r="E67" s="54">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="46"/>
-      <c r="C68" s="46"/>
-      <c r="E68" s="48"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="50"/>
+      <c r="E68" s="54"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -2650,10 +2684,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="45" t="s">
+      <c r="K75" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="45"/>
+      <c r="L75" s="49"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -2683,11 +2717,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="46">
+      <c r="K76" s="50">
         <f>SUM(B76:I76)</f>
         <v>96</v>
       </c>
-      <c r="L76" s="46"/>
+      <c r="L76" s="50"/>
       <c r="N76" s="13">
         <v>5</v>
       </c>
@@ -2715,20 +2749,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -2739,16 +2769,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2759,8 +2793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,60 +2823,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="65"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="63"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="68"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="66"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
-      <c r="H5" s="49" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="48"/>
+      <c r="H5" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="K5" s="49" t="s">
+      <c r="I5" s="48"/>
+      <c r="K5" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="51"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="48"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2920,37 +2954,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="45"/>
+      <c r="C9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="45"/>
+      <c r="H9" s="49"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="46">
+      <c r="B10" s="50">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>44.9</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="E10" s="55"/>
-      <c r="G10" s="46">
+      <c r="C10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="G10" s="50">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>21.1</v>
       </c>
-      <c r="H10" s="46"/>
+      <c r="H10" s="50"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="E11" s="56"/>
-      <c r="G11" s="46"/>
-      <c r="H11" s="46"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="E11" s="52"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -2986,35 +3020,35 @@
       <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="60"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="H17" s="49" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="H17" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
-      <c r="L17" s="45" t="s">
+      <c r="I17" s="47"/>
+      <c r="J17" s="48"/>
+      <c r="L17" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="45"/>
-      <c r="O17" s="45" t="s">
+      <c r="M17" s="49"/>
+      <c r="O17" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="45"/>
+      <c r="P17" s="49"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3044,17 +3078,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="46">
+      <c r="L18" s="50">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>70</v>
       </c>
-      <c r="M18" s="46"/>
-      <c r="O18" s="46">
+      <c r="M18" s="50"/>
+      <c r="O18" s="50">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>-20</v>
       </c>
-      <c r="P18" s="46"/>
-      <c r="R18" s="48">
+      <c r="P18" s="50"/>
+      <c r="R18" s="54">
         <v>4</v>
       </c>
     </row>
@@ -3081,11 +3115,11 @@
       <c r="J19" s="2">
         <v>12.5</v>
       </c>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="46"/>
-      <c r="R19" s="48"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="R19" s="54"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3110,56 +3144,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="63" t="s">
+      <c r="B23" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="65"/>
-      <c r="N23" s="46" t="s">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="63"/>
+      <c r="N23" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="46"/>
+      <c r="O23" s="50"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="66"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="68"/>
-      <c r="N24" s="46"/>
-      <c r="O24" s="46"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="66"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="47"/>
-      <c r="D26" s="47"/>
-      <c r="F26" s="47" t="s">
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="F26" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="45"/>
+      <c r="I26" s="45"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="49" t="s">
+      <c r="K26" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="51"/>
+      <c r="L26" s="48"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -3192,7 +3226,7 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="55"/>
+      <c r="N27" s="51"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -3216,7 +3250,7 @@
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="N28" s="56"/>
+      <c r="N28" s="52"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -3250,30 +3284,30 @@
       <c r="F32" s="58"/>
       <c r="G32" s="58"/>
       <c r="H32" s="58"/>
-      <c r="I32" s="59"/>
+      <c r="I32" s="67"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="60"/>
+      <c r="H33" s="60"/>
+      <c r="I33" s="68"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="47" t="s">
+      <c r="B35" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="47"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="51"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -3316,14 +3350,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="53"/>
-      <c r="F40" s="46" t="s">
+      <c r="C40" s="56"/>
+      <c r="F40" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="46"/>
+      <c r="G40" s="50"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3379,7 +3413,7 @@
       <c r="G43" s="2">
         <v>10</v>
       </c>
-      <c r="I43" s="45" t="s">
+      <c r="I43" s="49" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3394,7 +3428,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="45"/>
+      <c r="I44" s="49"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3557,48 +3591,48 @@
       <c r="S60" s="58"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="60"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="61"/>
-      <c r="I61" s="61"/>
-      <c r="J61" s="61"/>
-      <c r="K61" s="61"/>
-      <c r="L61" s="61"/>
-      <c r="M61" s="61"/>
-      <c r="N61" s="61"/>
-      <c r="O61" s="61"/>
-      <c r="P61" s="61"/>
-      <c r="Q61" s="61"/>
-      <c r="R61" s="61"/>
-      <c r="S61" s="61"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
+      <c r="E61" s="60"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="60"/>
+      <c r="H61" s="60"/>
+      <c r="I61" s="60"/>
+      <c r="J61" s="60"/>
+      <c r="K61" s="60"/>
+      <c r="L61" s="60"/>
+      <c r="M61" s="60"/>
+      <c r="N61" s="60"/>
+      <c r="O61" s="60"/>
+      <c r="P61" s="60"/>
+      <c r="Q61" s="60"/>
+      <c r="R61" s="60"/>
+      <c r="S61" s="60"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="47" t="s">
+      <c r="B63" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="47"/>
-      <c r="M63" s="47" t="s">
+      <c r="C63" s="45"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="45"/>
+      <c r="I63" s="45"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="45"/>
+      <c r="M63" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="47"/>
-      <c r="O63" s="47"/>
-      <c r="P63" s="47"/>
-      <c r="R63" s="47" t="s">
+      <c r="N63" s="45"/>
+      <c r="O63" s="45"/>
+      <c r="P63" s="45"/>
+      <c r="R63" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="47"/>
+      <c r="S63" s="45"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -3697,48 +3731,70 @@
       <c r="S65" s="2"/>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="J67" s="1" t="s">
+      <c r="J67" s="74" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="45" t="s">
+      <c r="B68" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="45"/>
+      <c r="C68" s="49"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="45" t="s">
+      <c r="G68" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="45"/>
-      <c r="J68" s="1">
+      <c r="H68" s="49"/>
+      <c r="J68" s="74">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="46">
+      <c r="B69" s="50">
         <f>SUM(B65:K65,M65:P65,R65:S65)+J68</f>
         <v>69</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="E69" s="48"/>
-      <c r="G69" s="46">
+      <c r="C69" s="50"/>
+      <c r="E69" s="54"/>
+      <c r="G69" s="50">
         <f>50-SUM(B65:K65,M65:P65,R65:S65,J68,K70)</f>
         <v>-19</v>
       </c>
-      <c r="H69" s="46"/>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="46"/>
-      <c r="C70" s="46"/>
-      <c r="E70" s="48"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="46"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="50"/>
+      <c r="E70" s="54"/>
+      <c r="G70" s="50"/>
+      <c r="H70" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -3755,28 +3811,6 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
zero exam mat3 - notes
</commit_message>
<xml_diff>
--- a/IoT-points-schedule.xlsx
+++ b/IoT-points-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jczec\Pulpit\IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C5E2B-3E73-4CB9-BAA8-8632F01A4937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C596683-D460-4BF4-8F8A-26DA46080460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{F85F5544-1FE8-4920-A5D4-192A98B113BD}"/>
   </bookViews>
   <sheets>
     <sheet name="I-semestr-24Z" sheetId="2" r:id="rId1"/>
@@ -1215,76 +1215,76 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1666,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5356A30-E1AA-4069-A4C8-FC0BE8204C56}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C42" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P70" sqref="P70"/>
     </sheetView>
   </sheetViews>
@@ -1732,23 +1732,23 @@
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
       <c r="I5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="49"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -1830,28 +1830,28 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="50"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="47">
+      <c r="B10" s="51">
         <f>_xlfn.CEILING.MATH(SUM(B7:G7,I7,K7:N7,P7),1,1)</f>
         <v>95</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="E10" s="56">
+      <c r="C10" s="51"/>
+      <c r="E10" s="52">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="E11" s="57"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="E11" s="53"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -1896,20 +1896,20 @@
       <c r="H15" s="45"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="F17" s="48" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="F17" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="J17" s="46" t="s">
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="J17" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="46"/>
+      <c r="K17" s="50"/>
       <c r="M17" s="9" t="s">
         <v>67</v>
       </c>
@@ -1933,12 +1933,12 @@
       <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="51">
         <f>SUM(B19:D19,F19:H19)</f>
         <v>19.7</v>
       </c>
-      <c r="K18" s="47"/>
-      <c r="M18" s="49">
+      <c r="K18" s="51"/>
+      <c r="M18" s="55">
         <v>3.5</v>
       </c>
     </row>
@@ -1955,9 +1955,9 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
-      <c r="M19" s="49"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="M19" s="55"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K20" s="1" t="s">
@@ -2015,20 +2015,20 @@
       <c r="K24" s="45"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="E26" s="50" t="s">
+      <c r="C26" s="46"/>
+      <c r="E26" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F26" s="51"/>
-      <c r="G26" s="52"/>
-      <c r="I26" s="48" t="s">
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
+      <c r="I26" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="48"/>
-      <c r="K26" s="48"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
       <c r="M26" s="10" t="s">
         <v>22</v>
       </c>
@@ -2063,12 +2063,12 @@
       <c r="K27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M27" s="55">
+      <c r="M27" s="54">
         <f>SUM(B28:C28,E28:G28,I28:K28)</f>
         <v>37.5</v>
       </c>
       <c r="N27" s="7"/>
-      <c r="O27" s="49">
+      <c r="O27" s="55">
         <v>4</v>
       </c>
       <c r="P27" s="8"/>
@@ -2098,9 +2098,9 @@
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
-      <c r="M28" s="55"/>
+      <c r="M28" s="54"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="49"/>
+      <c r="O28" s="55"/>
       <c r="P28" s="8"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2148,17 +2148,17 @@
       <c r="I33" s="45"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="F35" s="48" t="s">
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="F35" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="48"/>
-      <c r="H35" s="48"/>
-      <c r="I35" s="48"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
     </row>
@@ -2215,14 +2215,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="F40" s="47" t="s">
+      <c r="C40" s="57"/>
+      <c r="F40" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="47"/>
+      <c r="G40" s="51"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="G43" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I43" s="46" t="s">
+      <c r="I43" s="50" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2295,7 +2295,7 @@
       <c r="G44" s="2">
         <v>1</v>
       </c>
-      <c r="I44" s="46"/>
+      <c r="I44" s="50"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -2479,27 +2479,27 @@
       <c r="R59" s="45"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B61" s="48" t="s">
+      <c r="B61" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
-      <c r="K61" s="48"/>
-      <c r="M61" s="48" t="s">
+      <c r="C61" s="46"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
+      <c r="J61" s="46"/>
+      <c r="K61" s="46"/>
+      <c r="M61" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="N61" s="48"/>
-      <c r="O61" s="48"/>
-      <c r="Q61" s="48" t="s">
+      <c r="N61" s="46"/>
+      <c r="O61" s="46"/>
+      <c r="Q61" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="R61" s="48"/>
+      <c r="R61" s="46"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
@@ -2596,28 +2596,28 @@
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C66" s="46"/>
+      <c r="C66" s="50"/>
       <c r="E66" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B67" s="47">
+      <c r="B67" s="51">
         <f xml:space="preserve"> SUM(B63:K63,M63:O63,Q63:R63)</f>
         <v>81.7</v>
       </c>
-      <c r="C67" s="47"/>
-      <c r="E67" s="49">
+      <c r="C67" s="51"/>
+      <c r="E67" s="55">
         <v>4.5</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-      <c r="E68" s="49"/>
+      <c r="B68" s="51"/>
+      <c r="C68" s="51"/>
+      <c r="E68" s="55"/>
     </row>
     <row r="70" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
@@ -2688,10 +2688,10 @@
       <c r="I75" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K75" s="46" t="s">
+      <c r="K75" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="L75" s="46"/>
+      <c r="L75" s="50"/>
       <c r="N75" s="9" t="s">
         <v>67</v>
       </c>
@@ -2721,11 +2721,11 @@
       <c r="I76" s="2">
         <v>5</v>
       </c>
-      <c r="K76" s="47">
+      <c r="K76" s="51">
         <f>SUM(B76:I76)</f>
         <v>86</v>
       </c>
-      <c r="L76" s="47"/>
+      <c r="L76" s="51"/>
       <c r="N76" s="13">
         <v>4.5</v>
       </c>
@@ -2753,20 +2753,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B2:P3"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="B14:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B72:I73"/>
+    <mergeCell ref="K75:L75"/>
+    <mergeCell ref="K76:L76"/>
+    <mergeCell ref="B58:R59"/>
+    <mergeCell ref="B61:K61"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="Q61:R61"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C68"/>
+    <mergeCell ref="E67:E68"/>
     <mergeCell ref="I43:I44"/>
     <mergeCell ref="B23:K24"/>
     <mergeCell ref="B26:C26"/>
@@ -2777,16 +2773,20 @@
     <mergeCell ref="F35:I35"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B72:I73"/>
-    <mergeCell ref="K75:L75"/>
-    <mergeCell ref="K76:L76"/>
-    <mergeCell ref="B58:R59"/>
-    <mergeCell ref="B61:K61"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="Q61:R61"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C68"/>
-    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="B14:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="B2:P3"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2797,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C86BD6-21E5-4E44-BF61-9A65607E6D85}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K84" sqref="K84"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2827,60 +2827,60 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="66"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="64"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="67"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="68"/>
-      <c r="N3" s="68"/>
-      <c r="O3" s="68"/>
-      <c r="P3" s="69"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="67"/>
       <c r="R3" s="12"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="52"/>
-      <c r="H5" s="50" t="s">
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="H5" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="52"/>
-      <c r="K5" s="50" t="s">
+      <c r="I5" s="49"/>
+      <c r="K5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="51"/>
-      <c r="M5" s="51"/>
-      <c r="N5" s="52"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="49"/>
       <c r="P5" s="4" t="s">
         <v>74</v>
       </c>
@@ -2958,37 +2958,37 @@
       <c r="P7" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="46"/>
+      <c r="C9" s="50"/>
       <c r="E9" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="46"/>
+      <c r="H9" s="50"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="47">
+      <c r="B10" s="51">
         <f>SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>44.9</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="E10" s="56"/>
-      <c r="G10" s="47">
+      <c r="C10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="G10" s="51">
         <f>66-SUM(B7:F7,H7:I7,K7:N7,P7)</f>
         <v>21.1</v>
       </c>
-      <c r="H10" s="47"/>
+      <c r="H10" s="51"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="E11" s="57"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="51"/>
+      <c r="E11" s="53"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
@@ -3024,35 +3024,35 @@
       <c r="H14" s="59"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="61"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="H17" s="50" t="s">
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="H17" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="I17" s="51"/>
-      <c r="J17" s="52"/>
-      <c r="L17" s="46" t="s">
+      <c r="I17" s="48"/>
+      <c r="J17" s="49"/>
+      <c r="L17" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="46"/>
-      <c r="O17" s="46" t="s">
+      <c r="M17" s="50"/>
+      <c r="O17" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="P17" s="46"/>
+      <c r="P17" s="50"/>
       <c r="R17" s="9" t="s">
         <v>67</v>
       </c>
@@ -3082,17 +3082,17 @@
       <c r="J18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="47">
+      <c r="L18" s="51">
         <f>SUM(B19:F19,H19:J19)</f>
         <v>70</v>
       </c>
-      <c r="M18" s="47"/>
-      <c r="O18" s="47">
+      <c r="M18" s="51"/>
+      <c r="O18" s="51">
         <f>50-SUM(B19:F19,H19:J19)</f>
         <v>-20</v>
       </c>
-      <c r="P18" s="47"/>
-      <c r="R18" s="49">
+      <c r="P18" s="51"/>
+      <c r="R18" s="55">
         <v>4</v>
       </c>
     </row>
@@ -3119,11 +3119,11 @@
       <c r="J19" s="2">
         <v>12.5</v>
       </c>
-      <c r="L19" s="47"/>
-      <c r="M19" s="47"/>
-      <c r="O19" s="47"/>
-      <c r="P19" s="47"/>
-      <c r="R19" s="49"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="R19" s="55"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
@@ -3148,56 +3148,56 @@
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="58" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="65"/>
-      <c r="L23" s="66"/>
-      <c r="N23" s="47" t="s">
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="N23" s="51" t="s">
         <v>132</v>
       </c>
-      <c r="O23" s="47"/>
+      <c r="O23" s="51"/>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="67"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="69"/>
-      <c r="N24" s="47"/>
-      <c r="O24" s="47"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="F26" s="48" t="s">
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
+      <c r="F26" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="48"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="50" t="s">
+      <c r="K26" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="L26" s="52"/>
+      <c r="L26" s="49"/>
       <c r="N26" s="9" t="s">
         <v>67</v>
       </c>
@@ -3230,7 +3230,9 @@
       <c r="L27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N27" s="56"/>
+      <c r="N27" s="52">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
@@ -3252,9 +3254,13 @@
       <c r="I28" s="2">
         <v>5</v>
       </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="N28" s="57"/>
+      <c r="K28" s="2">
+        <v>5</v>
+      </c>
+      <c r="L28" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="N28" s="53"/>
     </row>
     <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
@@ -3288,30 +3294,30 @@
       <c r="F32" s="59"/>
       <c r="G32" s="59"/>
       <c r="H32" s="59"/>
-      <c r="I32" s="60"/>
+      <c r="I32" s="68"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="61"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="63"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="69"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="C35" s="48"/>
+      <c r="C35" s="46"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="52"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="49"/>
     </row>
     <row r="36" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
@@ -3354,14 +3360,14 @@
       <c r="O37" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="53" t="s">
+      <c r="B40" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="F40" s="47" t="s">
+      <c r="C40" s="57"/>
+      <c r="F40" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="47"/>
+      <c r="G40" s="51"/>
       <c r="I40" s="9" t="s">
         <v>22</v>
       </c>
@@ -3417,7 +3423,7 @@
       <c r="G43" s="2">
         <v>10</v>
       </c>
-      <c r="I43" s="46" t="s">
+      <c r="I43" s="50" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3432,7 +3438,7 @@
         <v>120</v>
       </c>
       <c r="G44" s="2"/>
-      <c r="I44" s="46"/>
+      <c r="I44" s="50"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
@@ -3595,48 +3601,48 @@
       <c r="S60" s="59"/>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="61"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="62"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="62"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="K61" s="62"/>
-      <c r="L61" s="62"/>
-      <c r="M61" s="62"/>
-      <c r="N61" s="62"/>
-      <c r="O61" s="62"/>
-      <c r="P61" s="62"/>
-      <c r="Q61" s="62"/>
-      <c r="R61" s="62"/>
-      <c r="S61" s="62"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="61"/>
+      <c r="D61" s="61"/>
+      <c r="E61" s="61"/>
+      <c r="F61" s="61"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="61"/>
+      <c r="I61" s="61"/>
+      <c r="J61" s="61"/>
+      <c r="K61" s="61"/>
+      <c r="L61" s="61"/>
+      <c r="M61" s="61"/>
+      <c r="N61" s="61"/>
+      <c r="O61" s="61"/>
+      <c r="P61" s="61"/>
+      <c r="Q61" s="61"/>
+      <c r="R61" s="61"/>
+      <c r="S61" s="61"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B63" s="48" t="s">
+      <c r="B63" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
-      <c r="J63" s="48"/>
-      <c r="K63" s="48"/>
-      <c r="M63" s="48" t="s">
+      <c r="C63" s="46"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="46"/>
+      <c r="M63" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="N63" s="48"/>
-      <c r="O63" s="48"/>
-      <c r="P63" s="48"/>
-      <c r="R63" s="48" t="s">
+      <c r="N63" s="46"/>
+      <c r="O63" s="46"/>
+      <c r="P63" s="46"/>
+      <c r="R63" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="S63" s="48"/>
+      <c r="S63" s="46"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
@@ -3740,43 +3746,65 @@
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="46"/>
+      <c r="C68" s="50"/>
       <c r="E68" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G68" s="46" t="s">
+      <c r="G68" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="H68" s="46"/>
+      <c r="H68" s="50"/>
       <c r="J68" s="39">
         <v>9</v>
       </c>
     </row>
     <row r="69" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B69" s="47">
+      <c r="B69" s="51">
         <f>SUM(B65:K65,M65:P65,R65:S65)+J68</f>
         <v>69</v>
       </c>
-      <c r="C69" s="47"/>
-      <c r="E69" s="49"/>
-      <c r="G69" s="47">
+      <c r="C69" s="51"/>
+      <c r="E69" s="55"/>
+      <c r="G69" s="51">
         <f>50-SUM(B65:K65,M65:P65,R65:S65,J68,K70)</f>
         <v>-19</v>
       </c>
-      <c r="H69" s="47"/>
+      <c r="H69" s="51"/>
     </row>
     <row r="70" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B70" s="47"/>
-      <c r="C70" s="47"/>
-      <c r="E70" s="49"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
+      <c r="B70" s="51"/>
+      <c r="C70" s="51"/>
+      <c r="E70" s="55"/>
+      <c r="G70" s="51"/>
+      <c r="H70" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="R63:S63"/>
+    <mergeCell ref="B32:I33"/>
+    <mergeCell ref="B63:K63"/>
+    <mergeCell ref="B60:S61"/>
+    <mergeCell ref="M63:P63"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="B23:L24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C70"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="G69:H70"/>
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="B14:H15"/>
     <mergeCell ref="K5:N5"/>
@@ -3793,28 +3821,6 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G10:H11"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C70"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H70"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="B23:L24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="R63:S63"/>
-    <mergeCell ref="B32:I33"/>
-    <mergeCell ref="B63:K63"/>
-    <mergeCell ref="B60:S61"/>
-    <mergeCell ref="M63:P63"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>